<commit_message>
Update user database file to reflect recent changes in user data structure
</commit_message>
<xml_diff>
--- a/userDB.xlsx
+++ b/userDB.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SK Chui\Desktop\tmp\20250319\tmpCode\my-250319_web\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SK Chui\Desktop\tmp\20250319\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1200869-31A4-4FDA-BB26-5BA3A8921005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF7E953-2DDE-4DF7-83EA-4753F4C1F808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1035" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{4783C5FF-8EC6-4DBC-AD77-05FDD494A060}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>username</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -59,6 +59,30 @@
   </si>
   <si>
     <t>teacher</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RCSS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -127,8 +151,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{534FDE86-829E-4356-938F-1D7FD2EF765A}" name="表格1" displayName="表格1" ref="A1:C2" totalsRowShown="0">
-  <autoFilter ref="A1:C2" xr:uid="{534FDE86-829E-4356-938F-1D7FD2EF765A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{534FDE86-829E-4356-938F-1D7FD2EF765A}" name="表格1" displayName="表格1" ref="A1:C7" totalsRowShown="0">
+  <autoFilter ref="A1:C7" xr:uid="{534FDE86-829E-4356-938F-1D7FD2EF765A}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{3453F8B3-B4CA-4083-810B-449F98188C8E}" name="username"/>
     <tableColumn id="2" xr3:uid="{7BD48662-0522-4F36-8A67-21FB1FF96FFA}" name="password"/>
@@ -455,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD1C26A7-6A8C-4479-ABA7-749F3BFCCB8A}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -489,6 +513,61 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add test Excel file creation and enhance error logging in user database loading
</commit_message>
<xml_diff>
--- a/userDB.xlsx
+++ b/userDB.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SK Chui\Desktop\tmp\20250319\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF7E953-2DDE-4DF7-83EA-4753F4C1F808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037D88D2-50EC-4C62-968F-988B6D78E851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1035" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{4783C5FF-8EC6-4DBC-AD77-05FDD494A060}"/>
   </bookViews>
   <sheets>
-    <sheet name="工作表1" sheetId="1" r:id="rId1"/>
+    <sheet name="userDB" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>username</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -51,14 +51,6 @@
   </si>
   <si>
     <t>jackchui123456</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>role</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>teacher</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -151,12 +143,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{534FDE86-829E-4356-938F-1D7FD2EF765A}" name="表格1" displayName="表格1" ref="A1:C7" totalsRowShown="0">
-  <autoFilter ref="A1:C7" xr:uid="{534FDE86-829E-4356-938F-1D7FD2EF765A}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{534FDE86-829E-4356-938F-1D7FD2EF765A}" name="表格1" displayName="表格1" ref="A1:B7" totalsRowShown="0">
+  <autoFilter ref="A1:B7" xr:uid="{534FDE86-829E-4356-938F-1D7FD2EF765A}"/>
+  <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{3453F8B3-B4CA-4083-810B-449F98188C8E}" name="username"/>
     <tableColumn id="2" xr3:uid="{7BD48662-0522-4F36-8A67-21FB1FF96FFA}" name="password"/>
-    <tableColumn id="3" xr3:uid="{AC67E5B3-2DA8-450A-8095-6E05E11FE65F}" name="role"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -479,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD1C26A7-6A8C-4479-ABA7-749F3BFCCB8A}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -491,80 +482,59 @@
     <col min="2" max="2" width="11.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
       <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update user database file to include recent user data modifications
</commit_message>
<xml_diff>
--- a/userDB.xlsx
+++ b/userDB.xlsx
@@ -2,80 +2,66 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SK Chui\Desktop\tmp\20250319\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SK Chui\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037D88D2-50EC-4C62-968F-988B6D78E851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33E7D37-23A4-4002-85E8-9873E620A387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1035" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{4783C5FF-8EC6-4DBC-AD77-05FDD494A060}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="userDB" sheetId="1" r:id="rId1"/>
+    <sheet name="Users" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>username</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>password</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>user123</t>
   </si>
   <si>
     <t>jackchui</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>jackchui123456</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>T1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>RCSS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>T2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>T3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>T4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>T5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -88,13 +74,12 @@
       <color theme="1"/>
       <name val="新細明體"/>
       <family val="2"/>
-      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="新細明體"/>
-      <family val="2"/>
+      <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
@@ -117,20 +102,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -142,19 +123,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{534FDE86-829E-4356-938F-1D7FD2EF765A}" name="表格1" displayName="表格1" ref="A1:B7" totalsRowShown="0">
-  <autoFilter ref="A1:B7" xr:uid="{534FDE86-829E-4356-938F-1D7FD2EF765A}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3453F8B3-B4CA-4083-810B-449F98188C8E}" name="username"/>
-    <tableColumn id="2" xr3:uid="{7BD48662-0522-4F36-8A67-21FB1FF96FFA}" name="password"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -164,44 +134,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -229,31 +199,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -281,23 +234,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -309,136 +245,180 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
+                <a:tint val="100000"/>
                 <a:shade val="100000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="phClr"/>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
     <a:lnDef>
       <a:spPr/>
       <a:bodyPr/>
@@ -460,27 +440,18 @@
     </a:lnDef>
   </a:objectDefaults>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD1C26A7-6A8C-4479-ABA7-749F3BFCCB8A}">
-  <dimension ref="A1:B7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="A5" sqref="A5:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.25" customWidth="1"/>
-    <col min="2" max="2" width="11.125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -511,38 +482,54 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
-        <v>5</v>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
+  <ignoredErrors>
+    <ignoredError sqref="A1:B4" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>